<commit_message>
changed the control id format of grievances
from interger to
PSGC+ 3 DIGIT USERUD+ 5 DIGIT SEQUNCE ID
</commit_message>
<xml_diff>
--- a/production/tbs/templates/grs_r1.xlsx
+++ b/production/tbs/templates/grs_r1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dev\OfflineGRS\production\tbs\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dev\offlinegrs\production\tbs\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE4E673-1B08-4366-A48A-FA13C0ABDC79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="R_A1" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <definedNames>
     <definedName name="the_named_cell">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>This sheet was hidden in the template, and it becomes visible.</t>
   </si>
@@ -156,11 +155,14 @@
       <t xml:space="preserve"> [onshow.a_coverage]</t>
     </r>
   </si>
+  <si>
+    <t>[a.docid;block=tbs:row]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -425,70 +427,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -501,6 +440,69 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -601,23 +603,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -653,23 +638,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -845,11 +813,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:M4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,72 +831,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
     </row>
     <row r="2" spans="1:15" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
     </row>
     <row r="3" spans="1:15" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
     </row>
     <row r="4" spans="1:15" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
     </row>
     <row r="5" spans="1:15" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12"/>
@@ -946,20 +914,20 @@
       <c r="M5" s="12"/>
     </row>
     <row r="6" spans="1:15" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="39"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
     </row>
@@ -980,93 +948,92 @@
       <c r="O7" s="8"/>
     </row>
     <row r="8" spans="1:15" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="33" t="s">
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
     </row>
     <row r="9" spans="1:15" s="9" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="34" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34" t="s">
+      <c r="J9" s="35"/>
+      <c r="K9" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
     </row>
     <row r="10" spans="1:15" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="28" t="s">
+      <c r="A10" s="30"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="28" t="s">
+      <c r="H10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="35" t="s">
+      <c r="I10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="35" t="s">
+      <c r="J10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="35" t="s">
+      <c r="K10" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="35" t="s">
+      <c r="L10" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="35" t="s">
+      <c r="M10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="N10" s="36" t="s">
+      <c r="N10" s="15" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <f>ROW()-9</f>
-        <v>2</v>
+      <c r="A11" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
@@ -1104,7 +1071,7 @@
       <c r="M11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N11" s="37" t="s">
+      <c r="N11" s="16" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1130,7 +1097,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>

</xml_diff>

<commit_message>
Revert "Revert "Additional feature:""
This reverts commit 3877bc26ae82e2c72bf3c1e6543a0d255d30f5cf.
</commit_message>
<xml_diff>
--- a/production/tbs/templates/grs_r1.xlsx
+++ b/production/tbs/templates/grs_r1.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7812"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7815"/>
   </bookViews>
   <sheets>
-    <sheet name="SAP" sheetId="3" r:id="rId1"/>
+    <sheet name="grs" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -62,10 +62,6 @@
     <t>DATE OF RESOLUTION</t>
   </si>
   <si>
-    <t>ACTIONS TAKEN
- (If referred, please specify name to whom grievance was referred)</t>
-  </si>
-  <si>
     <t>[a.PROVINCE;block=tbs:row]</t>
   </si>
   <si>
@@ -121,13 +117,39 @@
   </si>
   <si>
     <t>CLASSIFICATION</t>
+  </si>
+  <si>
+    <r>
+      <t>ACTIONS TAKEN
+ (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>If referred, please specify name to whom grievance was referred</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +195,13 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Candara"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -569,27 +598,25 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.5546875" customWidth="1"/>
+    <col min="5" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="9" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -604,9 +631,9 @@
       <c r="L1" s="11"/>
       <c r="M1" s="11"/>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" s="9" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -621,9 +648,9 @@
       <c r="L2" s="13"/>
       <c r="M2" s="13"/>
     </row>
-    <row r="3" spans="1:14" s="9" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" s="9" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
@@ -638,9 +665,9 @@
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
     </row>
-    <row r="4" spans="1:14" s="9" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" s="9" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
@@ -655,7 +682,7 @@
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
     </row>
-    <row r="5" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -667,9 +694,9 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -682,7 +709,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -694,7 +721,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="1:14" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
@@ -711,7 +738,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>2</v>
@@ -720,7 +747,7 @@
         <v>3</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>4</v>
@@ -738,48 +765,48 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="8" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="H9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="I9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="J9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="K9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="L9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="M9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="M9" s="7" t="s">
+      <c r="N9" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>